<commit_message>
completed sprint 6 actual
</commit_message>
<xml_diff>
--- a/teamOverview/sprintBacklog/sprint_6/Sprint_Burndown_6.xlsx
+++ b/teamOverview/sprintBacklog/sprint_6/Sprint_Burndown_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riaz\AppData\Local\Packages\CanonicalGroupLimited.UbuntuonWindows_79rhkp1fndgsc\LocalState\rootfs\root\Team10\teamOverview\sprintBacklog\sprint_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{27B2EF4E-9DC8-46FA-ADF7-C0128250DF46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{93B95110-91A6-40D8-9397-8FA60B2F8079}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6948" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>Provisional</t>
   </si>
@@ -160,6 +160,21 @@
   </si>
   <si>
     <t>Dann:3</t>
+  </si>
+  <si>
+    <t>52b</t>
+  </si>
+  <si>
+    <t>52c</t>
+  </si>
+  <si>
+    <t>52d</t>
+  </si>
+  <si>
+    <t>52e</t>
+  </si>
+  <si>
+    <t>54a</t>
   </si>
 </sst>
 </file>
@@ -480,19 +495,19 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -627,8 +642,8 @@
         <c:axId val="442376048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="33"/>
-          <c:min val="0"/>
+          <c:max val="35"/>
+          <c:min val="-5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1666,10 +1681,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1BB781-C491-4243-859C-AAD93AE5F06E}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2163,24 +2178,24 @@
         <v>31</v>
       </c>
       <c r="D15" s="1">
-        <f>C15-SUM(K25:K38)</f>
-        <v>31</v>
+        <f>C15-SUM(K25:K39)</f>
+        <v>29</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:H15" si="2">D15-SUM(L25:L38)</f>
-        <v>31</v>
+        <f t="shared" ref="E15:H15" si="2">D15-SUM(L25:L39)</f>
+        <v>29</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="23" spans="10:17" x14ac:dyDescent="0.3">
@@ -2208,16 +2223,134 @@
         <v>6</v>
       </c>
     </row>
+    <row r="25" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+    </row>
     <row r="27" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
       <c r="Q27" s="4"/>
     </row>
-    <row r="39" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J29" s="1">
+        <v>43</v>
+      </c>
+      <c r="M29" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J30" s="1">
+        <v>46</v>
+      </c>
+      <c r="M30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J31" s="1">
+        <v>47</v>
+      </c>
+      <c r="N31" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J32" s="1">
+        <v>50</v>
+      </c>
+      <c r="N32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="J33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O33" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="J34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N34" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="J35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N35" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="J36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="J37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="J38" s="1">
+        <v>54</v>
+      </c>
+      <c r="N38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="J40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K39" s="1">
-        <f>SUM(K25:O37)</f>
-        <v>0</v>
+      <c r="K40" s="1">
+        <f>SUM(K25:O39)</f>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised sprint 6 files
</commit_message>
<xml_diff>
--- a/teamOverview/sprintBacklog/sprint_6/Sprint_Burndown_6.xlsx
+++ b/teamOverview/sprintBacklog/sprint_6/Sprint_Burndown_6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riaz\AppData\Local\Packages\CanonicalGroupLimited.UbuntuonWindows_79rhkp1fndgsc\LocalState\rootfs\root\Team10\teamOverview\sprintBacklog\sprint_6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1478\Desktop\not_demo\Team10\teamOverview\sprintBacklog\sprint_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{93B95110-91A6-40D8-9397-8FA60B2F8079}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{81D9D46C-99B0-47EA-8A62-7F53E28D6083}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6948" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="14940" windowHeight="6945" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
   <si>
     <t>Provisional</t>
   </si>
@@ -162,19 +162,46 @@
     <t>Dann:3</t>
   </si>
   <si>
-    <t>52b</t>
-  </si>
-  <si>
-    <t>52c</t>
-  </si>
-  <si>
-    <t>52d</t>
-  </si>
-  <si>
-    <t>52e</t>
-  </si>
-  <si>
-    <t>54a</t>
+    <t>18a - David</t>
+  </si>
+  <si>
+    <t>21c - David</t>
+  </si>
+  <si>
+    <t>38a - Susan</t>
+  </si>
+  <si>
+    <t>38b - Susan</t>
+  </si>
+  <si>
+    <t>46 - Susan</t>
+  </si>
+  <si>
+    <t>47 - Susan</t>
+  </si>
+  <si>
+    <t>50 - Philip</t>
+  </si>
+  <si>
+    <t>52a - Dann</t>
+  </si>
+  <si>
+    <t>52b - Dann</t>
+  </si>
+  <si>
+    <t>52c - Dann</t>
+  </si>
+  <si>
+    <t>52d - Dann</t>
+  </si>
+  <si>
+    <t>52e - Dann</t>
+  </si>
+  <si>
+    <t>54 - David</t>
+  </si>
+  <si>
+    <t>54a - David</t>
   </si>
 </sst>
 </file>
@@ -501,13 +528,13 @@
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1354,7 +1381,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1681,33 +1708,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1BB781-C491-4243-859C-AAD93AE5F06E}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="5.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="5.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.21875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.21875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.109375" style="1" customWidth="1"/>
-    <col min="15" max="18" width="8.88671875" style="1"/>
-    <col min="19" max="19" width="8.88671875" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="13.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="1" customWidth="1"/>
+    <col min="15" max="18" width="8.85546875" style="1"/>
+    <col min="19" max="19" width="8.85546875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1715,7 +1740,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1765,7 +1790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1805,7 +1830,7 @@
       </c>
       <c r="S3" s="5"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1844,7 +1869,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1880,7 +1905,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1916,7 +1941,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1958,7 +1983,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2002,7 +2027,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J9" s="1">
         <v>6</v>
       </c>
@@ -2022,7 +2047,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -2045,7 +2070,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -2093,7 +2118,7 @@
       </c>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2122,6 +2147,9 @@
       <c r="K12" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="L12" s="1">
+        <v>52</v>
+      </c>
       <c r="M12" s="1">
         <v>3</v>
       </c>
@@ -2129,7 +2157,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J13" s="1">
         <v>10</v>
       </c>
@@ -2143,7 +2171,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -2169,7 +2197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
@@ -2178,32 +2206,32 @@
         <v>31</v>
       </c>
       <c r="D15" s="1">
-        <f>C15-SUM(K25:K39)</f>
+        <f>C15-SUM(K25:K38)</f>
         <v>29</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:H15" si="2">D15-SUM(L25:L39)</f>
+        <f>D15-SUM(L25:L38)</f>
         <v>29</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>E15-SUM(M25:M38)</f>
+        <v>24</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f>F15-SUM(N25:N38)</f>
+        <v>5</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="2"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="23" spans="10:17" x14ac:dyDescent="0.3">
+        <f>G15-SUM(O25:O38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J23" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="10:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J24" s="1" t="s">
         <v>1</v>
       </c>
@@ -2223,134 +2251,126 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="10:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J25" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="M25" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="10:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J26" s="1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="M26" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="10:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J27" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="K27" s="1">
         <v>1</v>
       </c>
       <c r="Q27" s="4"/>
     </row>
-    <row r="28" spans="10:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J28" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="K28" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="10:17" x14ac:dyDescent="0.3">
-      <c r="J29" s="1">
-        <v>43</v>
+    <row r="29" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J29" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="M29" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="10:17" x14ac:dyDescent="0.3">
-      <c r="J30" s="1">
-        <v>46</v>
-      </c>
-      <c r="M30" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="10:17" x14ac:dyDescent="0.3">
-      <c r="J31" s="1">
-        <v>47</v>
+    <row r="30" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N30" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J31" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="N31" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="10:17" x14ac:dyDescent="0.3">
-      <c r="J32" s="1">
-        <v>50</v>
-      </c>
-      <c r="N32" s="1">
+    <row r="32" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O32" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O33" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="10:15" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="N33" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J34" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="N34" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J35" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="N35" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J36" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="N36" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="10:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J37" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="N37" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="10:15" x14ac:dyDescent="0.3">
-      <c r="J38" s="1">
-        <v>54</v>
+    <row r="38" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J38" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="N38" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N39" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="10:15" x14ac:dyDescent="0.3">
-      <c r="J40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K40" s="1">
-        <f>SUM(K25:O39)</f>
-        <v>34</v>
+      <c r="K39" s="1">
+        <f>SUM(K25:O38)</f>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>